<commit_message>
Added PNG for animations Excel
</commit_message>
<xml_diff>
--- a/Other Files/Character Animations.xlsx
+++ b/Other Files/Character Animations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ch0m5 Database\ch0m5\Documents\GitHub\TheWitcher\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A764EC-457D-4FBF-8F1B-A82A7FB64E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3497B24-2AE4-4849-9107-78E37A98829A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="675" windowWidth="22305" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Geralt</t>
   </si>
@@ -121,6 +121,36 @@
   </si>
   <si>
     <t>All current Great Sword ones (already added)</t>
+  </si>
+  <si>
+    <t>Jaskier Abilities</t>
+  </si>
+  <si>
+    <t>Damage Line</t>
+  </si>
+  <si>
+    <t>Movement + Radius Blast</t>
+  </si>
+  <si>
+    <t>Concert</t>
+  </si>
+  <si>
+    <t>Sword and Shield Casting (Up and Down Smash)</t>
+  </si>
+  <si>
+    <t>Great Sword Casting (Up and Down Smash)</t>
+  </si>
+  <si>
+    <t>Moonwalk</t>
+  </si>
+  <si>
+    <t>Guitar Rock Finisher (CUSTOM)</t>
+  </si>
+  <si>
+    <t>Guitar Playing (Harder)</t>
+  </si>
+  <si>
+    <t>Stun Cone</t>
   </si>
 </sst>
 </file>
@@ -298,8 +328,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -314,6 +342,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,193 +627,219 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="A17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="A18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
+      <c r="A19" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
+      <c r="A20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>